<commit_message>
mode selector bug fixed
</commit_message>
<xml_diff>
--- a/back_log/Sprint1.xlsx
+++ b/back_log/Sprint1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fergus\Documents\GitHub\asteroid-designer-2\back_log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B016F436-63D7-42F9-A1A1-A7066D9E258B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B14CD09-7F92-4080-A0B5-FA148883CD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 07-03-2022" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="49">
   <si>
     <t>BACKLOG TASK &amp; ID</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>crater age and other propertys that PANGU offers</t>
+  </si>
+  <si>
+    <t>Sprint Backlog 3</t>
   </si>
 </sst>
 </file>
@@ -283,13 +286,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,18 +588,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="2:12" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
@@ -729,32 +732,32 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>0.5</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0</v>
-      </c>
-      <c r="I8" s="4">
-        <v>0</v>
-      </c>
-      <c r="J8" s="4">
-        <v>0</v>
-      </c>
-      <c r="K8" s="4"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3"/>
       <c r="L8" t="s">
         <v>34</v>
       </c>
@@ -1074,63 +1077,63 @@
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="5">
-        <v>1</v>
-      </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5">
-        <v>4</v>
-      </c>
-      <c r="F22" s="5">
-        <v>4</v>
-      </c>
-      <c r="G22" s="5">
-        <v>4</v>
-      </c>
-      <c r="H22" s="5">
-        <v>4</v>
-      </c>
-      <c r="I22" s="5">
-        <v>4</v>
-      </c>
-      <c r="J22" s="5">
+      <c r="C22" s="4">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4">
+        <v>4</v>
+      </c>
+      <c r="F22" s="4">
+        <v>4</v>
+      </c>
+      <c r="G22" s="4">
+        <v>4</v>
+      </c>
+      <c r="H22" s="4">
+        <v>4</v>
+      </c>
+      <c r="I22" s="4">
+        <v>4</v>
+      </c>
+      <c r="J22" s="4">
         <v>7</v>
       </c>
-      <c r="K22" s="5"/>
+      <c r="K22" s="4"/>
       <c r="L22" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="5">
-        <v>1</v>
-      </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5">
-        <v>2</v>
-      </c>
-      <c r="F23" s="5">
-        <v>2</v>
-      </c>
-      <c r="G23" s="5">
-        <v>2</v>
-      </c>
-      <c r="H23" s="5">
-        <v>2</v>
-      </c>
-      <c r="I23" s="5">
-        <v>2</v>
-      </c>
-      <c r="J23" s="5">
+      <c r="C23" s="4">
+        <v>1</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4">
+        <v>2</v>
+      </c>
+      <c r="F23" s="4">
+        <v>2</v>
+      </c>
+      <c r="G23" s="4">
+        <v>2</v>
+      </c>
+      <c r="H23" s="4">
+        <v>2</v>
+      </c>
+      <c r="I23" s="4">
+        <v>2</v>
+      </c>
+      <c r="J23" s="4">
         <v>7</v>
       </c>
-      <c r="K23" s="5"/>
+      <c r="K23" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1144,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F6E05B7-E04E-46DE-ABBF-E811B3E91D9C}">
   <dimension ref="B2:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K16" sqref="B2:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,18 +1157,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="2:12" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
@@ -1298,22 +1301,22 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="7">
-        <v>1</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7">
-        <v>3</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
+      <c r="C8" s="6">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6">
+        <v>3</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
       <c r="L8" t="s">
         <v>41</v>
       </c>
@@ -1409,7 +1412,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E13" s="2">
         <v>8</v>
@@ -1448,60 +1451,60 @@
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="6">
-        <v>2</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6">
-        <v>4</v>
-      </c>
-      <c r="F15" s="6">
+      <c r="C15" s="5">
+        <v>2</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5">
+        <v>4</v>
+      </c>
+      <c r="F15" s="5">
         <v>7</v>
       </c>
-      <c r="G15" s="6">
-        <v>0</v>
-      </c>
-      <c r="H15" s="6">
-        <v>0</v>
-      </c>
-      <c r="I15" s="6">
-        <v>0</v>
-      </c>
-      <c r="J15" s="6">
-        <v>0</v>
-      </c>
-      <c r="K15" s="6"/>
+      <c r="G15" s="5">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5">
+        <v>0</v>
+      </c>
+      <c r="K15" s="5"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="6">
-        <v>2</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6">
-        <v>4</v>
-      </c>
-      <c r="F16" s="6">
+      <c r="C16" s="5">
+        <v>2</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5">
+        <v>4</v>
+      </c>
+      <c r="F16" s="5">
         <v>7</v>
       </c>
-      <c r="G16" s="6">
-        <v>0</v>
-      </c>
-      <c r="H16" s="6">
-        <v>0</v>
-      </c>
-      <c r="I16" s="6">
-        <v>0</v>
-      </c>
-      <c r="J16" s="6">
-        <v>0</v>
-      </c>
-      <c r="K16" s="6"/>
+      <c r="G16" s="5">
+        <v>0</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <v>0</v>
+      </c>
+      <c r="K16" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1513,12 +1516,371 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31917C69-7D7A-4928-B5AB-80B1141C210D}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="85.85546875" customWidth="1"/>
+    <col min="3" max="11" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:11" ht="42.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="B2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" spans="2:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6">
+        <v>3</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="2">
+        <v>7</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>2.5</v>
+      </c>
+      <c r="F10">
+        <v>2.5</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>2.5</v>
+      </c>
+      <c r="F11">
+        <v>2.5</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="2">
+        <v>8</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="5">
+        <v>2</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5">
+        <v>4</v>
+      </c>
+      <c r="F15" s="5">
+        <v>7</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5">
+        <v>0</v>
+      </c>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="5">
+        <v>2</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5">
+        <v>4</v>
+      </c>
+      <c r="F16" s="5">
+        <v>7</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <v>0</v>
+      </c>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:K2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>